<commit_message>
i know i should not write code like this, but it wroks
</commit_message>
<xml_diff>
--- a/R/1.xlsx
+++ b/R/1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\personal\excel2ePrime\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1504C3F8-AF83-44F1-84B2-A98D0B0D90F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52A8E6A-C598-4854-8533-66A69F0B7CFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{64C9EB5E-7899-480B-AE8D-980B639420CD}"/>
   </bookViews>
@@ -37,21 +37,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>A</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>I have/has the doc/pen in my left hand</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>I have/has the haha/dog in my left hand</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>I have/has the dad/penmyass in my left hand</t>
+    <t>I have/has the doc/pen in my left/right hand</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -427,7 +419,7 @@
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -446,14 +438,10 @@
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:1" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
     <row r="13" spans="1:1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>

</xml_diff>